<commit_message>
Fixed changes on RDW.
</commit_message>
<xml_diff>
--- a/RDW/RDW.xlsx
+++ b/RDW/RDW.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/534a1defcf7f9d1a/Company Models CloudSave/RDW/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1550" documentId="8_{9D7C6FB3-E889-4C6A-A4F2-1ECF6CB88BB2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{EF3E3384-335A-4172-B985-8C4C6D3DEB2B}"/>
+  <xr:revisionPtr revIDLastSave="1589" documentId="8_{9D7C6FB3-E889-4C6A-A4F2-1ECF6CB88BB2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8094587F-0A64-417A-B62D-4E684A755C4D}"/>
   <bookViews>
-    <workbookView xWindow="12080" yWindow="5720" windowWidth="19450" windowHeight="13050" xr2:uid="{C970BFA8-84D0-4F74-AB89-871C65EF2168}"/>
+    <workbookView xWindow="18920" yWindow="5710" windowWidth="19450" windowHeight="13050" activeTab="2" xr2:uid="{C970BFA8-84D0-4F74-AB89-871C65EF2168}"/>
   </bookViews>
   <sheets>
     <sheet name="Main" sheetId="3" r:id="rId1"/>
@@ -249,7 +249,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="211" uniqueCount="195">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="217" uniqueCount="201">
   <si>
     <t>Quarter</t>
   </si>
@@ -950,6 +950,24 @@
   </si>
   <si>
     <t>Redwire Rollout Solar Array (ROSA)</t>
+  </si>
+  <si>
+    <t>Analyst Estimates</t>
+  </si>
+  <si>
+    <t>EPS - Actual</t>
+  </si>
+  <si>
+    <t>EPS - Forecast</t>
+  </si>
+  <si>
+    <t>Surprise %</t>
+  </si>
+  <si>
+    <t>Notes</t>
+  </si>
+  <si>
+    <t>- First FCF positive quarter Q223</t>
   </si>
 </sst>
 </file>
@@ -1140,7 +1158,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="49">
+  <cellXfs count="51">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -1192,6 +1210,8 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="10" fontId="4" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="10" fontId="4" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1336,10 +1356,10 @@
     <v>4.58</v>
     <v>1.67</v>
     <v>1.522</v>
-    <v>-0.65</v>
-    <v>5.7576000000000002E-2</v>
-    <v>-0.15776699999999999</v>
-    <v>0.19</v>
+    <v>0.06</v>
+    <v>2.3820999999999998E-2</v>
+    <v>1.8182E-2</v>
+    <v>7.9799999999999996E-2</v>
     <v>USD</v>
     <v>Redwire Corporation develops and manufactures mission-critical space solutions and high-reliability components for the space economy, with intellectual property for solar power generation, in-space 3D printing and manufacturing, avionics, critical components, sensors, digital engineering and space-based biotechnology. The Company’s products and solutions include antennas, satellite technology, space-qualified sensors, deployable space structure, berthing and docking equipment, and space-enabled manufacturing payloads. It offers enterprise software suite that enables advanced digital engineering and generation of high fidelity, interactive modeling and simulations of individual components, entire spacecraft and full constellations in a cloud-based software-as-a-service (SaaS) business model. Its technologies include roll out solar array (ROSA) systems; human-rated camera systems; in-space servicing, assembly and manufacturing (ISAM) products, and advanced payload adapters.</v>
     <v>700</v>
@@ -1347,24 +1367,24 @@
     <v>XNYS</v>
     <v>XNYS</v>
     <v>8226 Philips Highway, Suite 101, Suite 101, JACKSONVILLE, FL, 32256 US</v>
-    <v>4.2698999999999998</v>
+    <v>3.7</v>
     <v>Aerospace &amp; Defense</v>
     <v>Stock</v>
-    <v>45184.989039282031</v>
+    <v>45187.996062279686</v>
     <v>0</v>
-    <v>3.3</v>
-    <v>213726300</v>
+    <v>3.32</v>
+    <v>217612180</v>
     <v>REDWIRE CORPORATION</v>
     <v>REDWIRE CORPORATION</v>
-    <v>4.12</v>
-    <v>4.12</v>
-    <v>3.47</v>
-    <v>3.49</v>
+    <v>3.4</v>
+    <v>3.3</v>
+    <v>3.36</v>
+    <v>3.4298000000000002</v>
     <v>64765530</v>
     <v>RDW</v>
     <v>REDWIRE CORPORATION (XNYS:RDW)</v>
-    <v>1022785</v>
-    <v>182822</v>
+    <v>702896</v>
+    <v>218141</v>
     <v>2021</v>
   </rv>
   <rv s="2">
@@ -1526,9 +1546,9 @@
       <v>at close</v>
       <v>from previous close</v>
       <v>from previous close</v>
-      <v>Source: Nasdaq</v>
+      <v>Source: Nasdaq Last Sale</v>
       <v>GMT</v>
-      <v>Delayed 15 minutes</v>
+      <v>Real-Time Nasdaq Last Sale</v>
       <v>from close</v>
       <v>from close</v>
     </spb>
@@ -1945,13 +1965,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{88F90BA7-A564-46F1-9574-0FAA5750F1B7}">
-  <dimension ref="A1:B7"/>
+  <dimension ref="A1:B13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O7" sqref="O7"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="9.453125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" t="e" vm="1">
@@ -1964,7 +1987,7 @@
       </c>
       <c r="B2" s="31">
         <f t="array" ref="B2">_FV(A1,"Price")</f>
-        <v>3.47</v>
+        <v>3.36</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
@@ -1982,7 +2005,7 @@
       </c>
       <c r="B4" s="32">
         <f>B2*B3</f>
-        <v>224736.3891</v>
+        <v>217612.1808</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.35">
@@ -2008,7 +2031,20 @@
       </c>
       <c r="B7" s="32">
         <f>B4-B5+B6</f>
-        <v>307014.38910000003</v>
+        <v>299890.18079999997</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A12" s="2" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A13" s="3">
+        <v>45187</v>
+      </c>
+      <c r="B13" s="6" t="s">
+        <v>200</v>
       </c>
     </row>
   </sheetData>
@@ -2600,13 +2636,13 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A4250126-BCEC-4955-9E0E-CDA1E5117D90}">
-  <dimension ref="B1:AI119"/>
+  <dimension ref="B1:AI122"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="2" ySplit="7" topLeftCell="I59" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="2" ySplit="7" topLeftCell="J89" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
-      <selection pane="bottomRight" activeCell="V91" sqref="V91"/>
+      <selection pane="bottomRight" activeCell="S96" sqref="S96"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -4094,7 +4130,10 @@
     <row r="36" spans="2:35" s="7" customFormat="1" x14ac:dyDescent="0.35">
       <c r="I36" s="21"/>
       <c r="M36" s="21"/>
-      <c r="Q36" s="21"/>
+      <c r="Q36" s="21">
+        <f>Q32/Q35</f>
+        <v>-0.11291115048326143</v>
+      </c>
     </row>
     <row r="37" spans="2:35" s="7" customFormat="1" x14ac:dyDescent="0.35">
       <c r="I37" s="21"/>
@@ -7786,10 +7825,70 @@
       <c r="M118" s="43"/>
       <c r="Q118" s="43"/>
     </row>
-    <row r="119" spans="2:35" s="42" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="I119" s="43"/>
-      <c r="M119" s="43"/>
-      <c r="Q119" s="43"/>
+    <row r="119" spans="2:35" s="49" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="B119" s="49" t="s">
+        <v>195</v>
+      </c>
+      <c r="I119" s="50"/>
+      <c r="M119" s="50"/>
+      <c r="Q119" s="50"/>
+    </row>
+    <row r="120" spans="2:35" x14ac:dyDescent="0.35">
+      <c r="B120" t="s">
+        <v>196</v>
+      </c>
+      <c r="O120">
+        <v>-0.12</v>
+      </c>
+      <c r="P120">
+        <v>-0.13</v>
+      </c>
+      <c r="Q120" s="17">
+        <v>-0.18</v>
+      </c>
+      <c r="R120">
+        <v>-0.16</v>
+      </c>
+    </row>
+    <row r="121" spans="2:35" x14ac:dyDescent="0.35">
+      <c r="B121" t="s">
+        <v>197</v>
+      </c>
+      <c r="O121">
+        <v>-0.16</v>
+      </c>
+      <c r="P121">
+        <v>-0.43</v>
+      </c>
+      <c r="Q121" s="17">
+        <v>-0.18</v>
+      </c>
+      <c r="R121">
+        <v>-0.16</v>
+      </c>
+    </row>
+    <row r="122" spans="2:35" s="42" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="B122" s="42" t="s">
+        <v>198</v>
+      </c>
+      <c r="I122" s="43"/>
+      <c r="M122" s="43"/>
+      <c r="O122" s="42">
+        <f>(O121-O120)/ABS(O120)</f>
+        <v>-0.33333333333333343</v>
+      </c>
+      <c r="P122" s="42">
+        <f>(P121-P120)/ABS(P120)</f>
+        <v>-2.3076923076923075</v>
+      </c>
+      <c r="Q122" s="43">
+        <f>(Q121-Q120)/ABS(Q120)</f>
+        <v>0</v>
+      </c>
+      <c r="R122" s="42">
+        <f>(R121-R120)/ABS(R120)</f>
+        <v>0</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Made minor changes to formatting.
</commit_message>
<xml_diff>
--- a/RDW/RDW.xlsx
+++ b/RDW/RDW.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/534a1defcf7f9d1a/Company Models CloudSave/RDW/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1593" documentId="8_{9D7C6FB3-E889-4C6A-A4F2-1ECF6CB88BB2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E7696060-A03D-4E30-90FA-8992A0CF5053}"/>
+  <xr:revisionPtr revIDLastSave="1597" documentId="8_{9D7C6FB3-E889-4C6A-A4F2-1ECF6CB88BB2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{BE380FB9-641D-47AA-B9DA-B8522E84505A}"/>
   <bookViews>
-    <workbookView xWindow="44280" yWindow="3090" windowWidth="26720" windowHeight="17120" activeTab="1" xr2:uid="{C970BFA8-84D0-4F74-AB89-871C65EF2168}"/>
+    <workbookView xWindow="45960" yWindow="2890" windowWidth="26720" windowHeight="17120" activeTab="1" xr2:uid="{C970BFA8-84D0-4F74-AB89-871C65EF2168}"/>
   </bookViews>
   <sheets>
     <sheet name="Main" sheetId="3" r:id="rId1"/>
@@ -1356,10 +1356,8 @@
     <v>4.58</v>
     <v>1.67</v>
     <v>1.522</v>
-    <v>-0.19</v>
-    <v>2.9090999999999999E-2</v>
-    <v>-6.4626000000000003E-2</v>
-    <v>0.08</v>
+    <v>0</v>
+    <v>0</v>
     <v>USD</v>
     <v>Redwire Corporation develops and manufactures mission-critical space solutions and high-reliability components for the space economy, with intellectual property for solar power generation, in-space 3D printing and manufacturing, avionics, critical components, sensors, digital engineering and space-based biotechnology. The Company’s products and solutions include antennas, satellite technology, space-qualified sensors, deployable space structure, berthing and docking equipment, and space-enabled manufacturing payloads. It offers enterprise software suite that enables advanced digital engineering and generation of high fidelity, interactive modeling and simulations of individual components, entire spacecraft and full constellations in a cloud-based software-as-a-service (SaaS) business model. Its technologies include roll out solar array (ROSA) systems; human-rated camera systems; in-space servicing, assembly and manufacturing (ISAM) products, and advanced payload adapters.</v>
     <v>700</v>
@@ -1367,24 +1365,23 @@
     <v>XNYS</v>
     <v>XNYS</v>
     <v>8226 Philips Highway, Suite 101, Suite 101, JACKSONVILLE, FL, 32256 US</v>
-    <v>2.9182000000000001</v>
+    <v>2.95</v>
     <v>Aerospace &amp; Defense</v>
     <v>Stock</v>
-    <v>45194.833797916406</v>
+    <v>45197.958333367969</v>
     <v>0</v>
-    <v>2.64</v>
-    <v>178105207</v>
+    <v>2.82</v>
+    <v>185877071</v>
     <v>REDWIRE CORPORATION</v>
     <v>REDWIRE CORPORATION</v>
-    <v>2.89</v>
-    <v>2.94</v>
-    <v>2.75</v>
-    <v>2.83</v>
+    <v>2.9</v>
+    <v>2.87</v>
+    <v>2.87</v>
     <v>64765530</v>
     <v>RDW</v>
     <v>REDWIRE CORPORATION (XNYS:RDW)</v>
-    <v>363338</v>
-    <v>249610</v>
+    <v>100471</v>
+    <v>257377</v>
     <v>2021</v>
   </rv>
   <rv s="2">
@@ -1415,9 +1412,7 @@
     <k n="52 week low"/>
     <k n="Beta"/>
     <k n="Change"/>
-    <k n="Change % (Extended hours)"/>
     <k n="Change (%)"/>
-    <k n="Change (Extended hours)"/>
     <k n="Currency" t="s"/>
     <k n="Description" t="s"/>
     <k n="Employees"/>
@@ -1437,7 +1432,6 @@
     <k n="Open"/>
     <k n="Previous close"/>
     <k n="Price"/>
-    <k n="Price (Extended hours)"/>
     <k n="Shares outstanding"/>
     <k n="Ticker symbol" t="s"/>
     <k n="UniqueName" t="s"/>
@@ -1454,7 +1448,7 @@
 <file path=xl/richData/rdsupportingpropertybag.xml><?xml version="1.0" encoding="utf-8"?>
 <supportingPropertyBags xmlns="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2">
   <spbArrays count="1">
-    <a count="44">
+    <a count="41">
       <v t="s">%EntityServiceId</v>
       <v t="s">_Format</v>
       <v t="s">%IsRefreshable</v>
@@ -1465,16 +1459,13 @@
       <v t="s">Name</v>
       <v t="s">_SubLabel</v>
       <v t="s">Price</v>
-      <v t="s">Price (Extended hours)</v>
       <v t="s">Exchange</v>
       <v t="s">Official name</v>
       <v t="s">Last trade time</v>
       <v t="s">Ticker symbol</v>
       <v t="s">Exchange abbreviation</v>
       <v t="s">Change</v>
-      <v t="s">Change (Extended hours)</v>
       <v t="s">Change (%)</v>
-      <v t="s">Change % (Extended hours)</v>
       <v t="s">Currency</v>
       <v t="s">Previous close</v>
       <v t="s">Open</v>
@@ -1538,19 +1529,13 @@
       <v>8</v>
       <v>9</v>
       <v>4</v>
-      <v>1</v>
-      <v>1</v>
-      <v>5</v>
     </spb>
     <spb s="4">
-      <v>at close</v>
+      <v>Delayed 15 minutes</v>
       <v>from previous close</v>
       <v>from previous close</v>
-      <v>Source: Nasdaq Last Sale</v>
+      <v>Source: Nasdaq</v>
       <v>GMT</v>
-      <v>Real-Time Nasdaq Last Sale</v>
-      <v>from close</v>
-      <v>from close</v>
     </spb>
   </spbData>
 </supportingPropertyBags>
@@ -1594,9 +1579,6 @@
     <k n="Year incorporated" t="i"/>
     <k n="`%EntityServiceId" t="i"/>
     <k n="Shares outstanding" t="i"/>
-    <k n="Price (Extended hours)" t="i"/>
-    <k n="Change (Extended hours)" t="i"/>
-    <k n="Change % (Extended hours)" t="i"/>
   </s>
   <s>
     <k n="Price" t="s"/>
@@ -1604,9 +1586,6 @@
     <k n="Change (%)" t="s"/>
     <k n="ExchangeID" t="s"/>
     <k n="Last trade time" t="s"/>
-    <k n="Price (Extended hours)" t="s"/>
-    <k n="Change (Extended hours)" t="s"/>
-    <k n="Change % (Extended hours)" t="s"/>
   </s>
 </spbStructures>
 </file>
@@ -1987,7 +1966,7 @@
       </c>
       <c r="B2" s="31">
         <f t="array" ref="B2">_FV(A1,"Price")</f>
-        <v>2.75</v>
+        <v>2.87</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
@@ -2005,7 +1984,7 @@
       </c>
       <c r="B4" s="32">
         <f>B2*B3</f>
-        <v>178105.20749999999</v>
+        <v>185877.0711</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.35">
@@ -2031,7 +2010,7 @@
       </c>
       <c r="B7" s="32">
         <f>B4-B5+B6</f>
-        <v>260383.20749999999</v>
+        <v>268155.0711</v>
       </c>
     </row>
     <row r="12" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.35">
@@ -2058,7 +2037,7 @@
   <dimension ref="A1:Z111"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:A6"/>
+      <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>